<commit_message>
work on network visualization, density, transitivity
</commit_message>
<xml_diff>
--- a/env_meta_data.xlsx
+++ b/env_meta_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chanyaaaas/Documents/External Norm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chanyaaaas/Documents/environmental_dispute/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375EA56F-4E62-414D-8B85-612C3AFC1CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5D91C7-5C74-DD40-8D45-330349CA0271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="36720" windowHeight="20860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1031,12 +1031,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1051,8 +1057,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,14 +1358,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="3" max="3" width="62.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="14.83203125" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -1377,7 +1388,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1389,16 +1400,16 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="N1" t="s">
@@ -1436,7 +1447,7 @@
       <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>1996</v>
       </c>
       <c r="H2">
@@ -1445,13 +1456,13 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="1">
         <v>1</v>
       </c>
       <c r="U2">
@@ -1468,16 +1479,16 @@
       <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>1998</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>0</v>
       </c>
       <c r="U3">
@@ -1494,16 +1505,16 @@
       <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>1998</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="1">
         <v>0</v>
       </c>
       <c r="U4">
@@ -1520,13 +1531,13 @@
       <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>1997</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="1">
         <v>0</v>
       </c>
       <c r="U5">
@@ -1543,13 +1554,13 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>1998</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="1">
         <v>0</v>
       </c>
       <c r="U6">
@@ -1566,13 +1577,13 @@
       <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>1998</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="1">
         <v>0</v>
       </c>
       <c r="U7">
@@ -1589,13 +1600,13 @@
       <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>1998</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="1">
         <v>0</v>
       </c>
       <c r="U8">
@@ -1612,13 +1623,13 @@
       <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>1997</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="1">
         <v>0</v>
       </c>
       <c r="U9">
@@ -1635,13 +1646,13 @@
       <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>1997</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="1">
         <v>0</v>
       </c>
       <c r="U10">
@@ -1658,13 +1669,13 @@
       <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>2001</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="1">
         <v>0</v>
       </c>
       <c r="N11" t="s">
@@ -1684,13 +1695,13 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>2000</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="1">
         <v>0</v>
       </c>
       <c r="U12">
@@ -1707,13 +1718,13 @@
       <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>2003</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="1">
         <v>0</v>
       </c>
       <c r="U13">
@@ -1730,13 +1741,13 @@
       <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>2005</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="1">
         <v>0</v>
       </c>
       <c r="U14">
@@ -1753,13 +1764,13 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>2005</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="1">
         <v>0</v>
       </c>
       <c r="U15">
@@ -1776,13 +1787,13 @@
       <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="1">
         <v>2006</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="1">
         <v>0</v>
       </c>
       <c r="U16">
@@ -1799,13 +1810,13 @@
       <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>2009</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="1">
         <v>0</v>
       </c>
       <c r="U17">
@@ -1822,16 +1833,16 @@
       <c r="C18" t="s">
         <v>42</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>2014</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="1">
         <v>0</v>
       </c>
       <c r="N18" t="s">
@@ -1851,13 +1862,13 @@
       <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>2012</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="U19">
@@ -1874,13 +1885,13 @@
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>2012</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="U20">
@@ -1897,13 +1908,13 @@
       <c r="C21" t="s">
         <v>45</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>2011</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="U21">
@@ -1920,13 +1931,13 @@
       <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>2011</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="1">
         <v>0</v>
       </c>
       <c r="U22">
@@ -1943,13 +1954,13 @@
       <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>2012</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="1">
         <v>0</v>
       </c>
       <c r="U23">
@@ -1966,13 +1977,13 @@
       <c r="C24" t="s">
         <v>48</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>2016</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="1">
         <v>0</v>
       </c>
       <c r="U24">
@@ -1989,13 +2000,13 @@
       <c r="C25" t="s">
         <v>49</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>2016</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="1">
         <v>0</v>
       </c>
       <c r="U25">
@@ -2012,7 +2023,7 @@
       <c r="C26" t="s">
         <v>52</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>2006</v>
       </c>
       <c r="G26" t="s">
@@ -2021,10 +2032,10 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>0</v>
       </c>
       <c r="U26">
@@ -2041,7 +2052,7 @@
       <c r="C27" t="s">
         <v>56</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="1">
         <v>2016</v>
       </c>
       <c r="G27" t="s">
@@ -2050,10 +2061,10 @@
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="1">
         <v>0</v>
       </c>
       <c r="U27">
@@ -2070,7 +2081,7 @@
       <c r="C28" t="s">
         <v>58</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>2018</v>
       </c>
       <c r="G28" t="s">
@@ -2079,10 +2090,10 @@
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="1">
         <v>0</v>
       </c>
       <c r="U28">
@@ -2099,7 +2110,7 @@
       <c r="C29" t="s">
         <v>60</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>2017</v>
       </c>
       <c r="G29" t="s">
@@ -2108,13 +2119,13 @@
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
+      <c r="L29" s="1">
+        <v>0</v>
+      </c>
+      <c r="M29" s="1">
         <v>0</v>
       </c>
       <c r="N29" t="s">
@@ -2149,13 +2160,13 @@
       <c r="C30" t="s">
         <v>66</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="1">
         <v>1971</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="1">
         <v>0</v>
       </c>
       <c r="U30">
@@ -2172,13 +2183,13 @@
       <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>1978</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="1">
         <v>0</v>
       </c>
       <c r="U31">
@@ -2195,13 +2206,13 @@
       <c r="C32" t="s">
         <v>71</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="1">
         <v>1925</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="1">
         <v>0</v>
       </c>
       <c r="U32">
@@ -2218,13 +2229,13 @@
       <c r="C33" t="s">
         <v>73</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>1926</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="1">
         <v>0</v>
       </c>
       <c r="U33">
@@ -2238,7 +2249,7 @@
       <c r="B34" t="s">
         <v>75</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>2004</v>
       </c>
       <c r="G34" t="s">
@@ -2250,7 +2261,7 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="1">
         <v>0</v>
       </c>
       <c r="U34">
@@ -2264,7 +2275,7 @@
       <c r="B35" t="s">
         <v>76</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>2005</v>
       </c>
       <c r="G35" t="s">
@@ -2276,7 +2287,7 @@
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="L35">
+      <c r="L35" s="1">
         <v>0</v>
       </c>
       <c r="U35">
@@ -2290,7 +2301,7 @@
       <c r="B36" t="s">
         <v>77</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>2011</v>
       </c>
       <c r="G36" t="s">
@@ -2302,7 +2313,7 @@
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="L36">
+      <c r="L36" s="1">
         <v>0</v>
       </c>
       <c r="U36">
@@ -2319,7 +2330,7 @@
       <c r="C37" t="s">
         <v>80</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>2002</v>
       </c>
       <c r="G37" t="s">
@@ -2331,7 +2342,7 @@
       <c r="I37">
         <v>1</v>
       </c>
-      <c r="L37">
+      <c r="L37" s="1">
         <v>0</v>
       </c>
       <c r="U37">
@@ -2348,13 +2359,13 @@
       <c r="C38" t="s">
         <v>83</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>1986</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="L38">
+      <c r="L38" s="1">
         <v>0</v>
       </c>
       <c r="U38">
@@ -2371,7 +2382,7 @@
       <c r="C39" t="s">
         <v>86</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>1997</v>
       </c>
       <c r="G39" t="s">
@@ -2380,10 +2391,10 @@
       <c r="H39">
         <v>0</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L39">
+      <c r="L39" s="1">
         <v>0</v>
       </c>
       <c r="S39" t="s">
@@ -2403,7 +2414,7 @@
       <c r="C40" t="s">
         <v>90</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>2000</v>
       </c>
       <c r="G40" t="s">
@@ -2412,10 +2423,10 @@
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L40">
+      <c r="L40" s="1">
         <v>0</v>
       </c>
       <c r="S40" t="s">
@@ -2435,7 +2446,7 @@
       <c r="C41" t="s">
         <v>92</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>2000</v>
       </c>
       <c r="G41" t="s">
@@ -2444,10 +2455,10 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L41">
+      <c r="L41" s="1">
         <v>0</v>
       </c>
       <c r="S41" t="s">
@@ -2467,7 +2478,7 @@
       <c r="C42" t="s">
         <v>94</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>2001</v>
       </c>
       <c r="G42" t="s">
@@ -2476,10 +2487,10 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="1">
         <v>0</v>
       </c>
       <c r="S42" t="s">
@@ -2499,7 +2510,7 @@
       <c r="C43" t="s">
         <v>97</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>2001</v>
       </c>
       <c r="G43" t="s">
@@ -2508,10 +2519,10 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="1">
         <v>0</v>
       </c>
       <c r="S43" t="s">
@@ -2531,7 +2542,7 @@
       <c r="C44" t="s">
         <v>100</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>2002</v>
       </c>
       <c r="G44" t="s">
@@ -2540,10 +2551,10 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="1">
         <v>0</v>
       </c>
       <c r="S44" t="s">
@@ -2563,7 +2574,7 @@
       <c r="C45" t="s">
         <v>102</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>2004</v>
       </c>
       <c r="G45" t="s">
@@ -2572,10 +2583,10 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="J45" t="s">
+      <c r="J45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="1">
         <v>0</v>
       </c>
       <c r="S45" t="s">
@@ -2595,7 +2606,7 @@
       <c r="C46" t="s">
         <v>104</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>2007</v>
       </c>
       <c r="G46" t="s">
@@ -2604,10 +2615,10 @@
       <c r="H46">
         <v>0</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L46">
+      <c r="L46" s="1">
         <v>0</v>
       </c>
       <c r="S46" t="s">
@@ -2627,7 +2638,7 @@
       <c r="C47" t="s">
         <v>106</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>2007</v>
       </c>
       <c r="G47" t="s">
@@ -2636,10 +2647,10 @@
       <c r="H47">
         <v>0</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L47">
+      <c r="L47" s="1">
         <v>0</v>
       </c>
       <c r="S47" t="s">
@@ -2659,7 +2670,7 @@
       <c r="C48" t="s">
         <v>109</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>1987</v>
       </c>
       <c r="H48">
@@ -2668,13 +2679,13 @@
       <c r="I48">
         <v>0</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J48" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L48">
-        <v>0</v>
-      </c>
-      <c r="M48">
+      <c r="L48" s="1">
+        <v>0</v>
+      </c>
+      <c r="M48" s="1">
         <v>0</v>
       </c>
       <c r="U48">
@@ -2697,7 +2708,7 @@
       <c r="E49" t="s">
         <v>113</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>1989</v>
       </c>
       <c r="H49">
@@ -2706,13 +2717,13 @@
       <c r="I49">
         <v>0</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J49" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
+      <c r="L49" s="1">
+        <v>0</v>
+      </c>
+      <c r="M49" s="1">
         <v>0</v>
       </c>
       <c r="U49">
@@ -2735,7 +2746,7 @@
       <c r="E50" t="s">
         <v>112</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>1990</v>
       </c>
       <c r="G50" t="s">
@@ -2747,13 +2758,13 @@
       <c r="I50">
         <v>0</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J50" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
+      <c r="L50" s="1">
+        <v>0</v>
+      </c>
+      <c r="M50" s="1">
         <v>0</v>
       </c>
       <c r="U50">
@@ -2776,7 +2787,7 @@
       <c r="E51" t="s">
         <v>119</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="1">
         <v>1996</v>
       </c>
       <c r="G51" t="s">
@@ -2788,16 +2799,16 @@
       <c r="I51">
         <v>1</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K51" t="s">
         <v>24</v>
       </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-      <c r="M51">
+      <c r="L51" s="1">
+        <v>1</v>
+      </c>
+      <c r="M51" s="1">
         <v>1</v>
       </c>
       <c r="N51" t="s">
@@ -2838,7 +2849,7 @@
       <c r="E52" t="s">
         <v>124</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>1998</v>
       </c>
       <c r="G52" t="s">
@@ -2850,16 +2861,16 @@
       <c r="I52">
         <v>1</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J52" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K52" t="s">
         <v>125</v>
       </c>
-      <c r="L52">
+      <c r="L52" s="1">
         <v>6</v>
       </c>
-      <c r="M52">
+      <c r="M52" s="1">
         <v>1</v>
       </c>
       <c r="N52" t="s">
@@ -2900,7 +2911,7 @@
       <c r="E53" t="s">
         <v>129</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="1">
         <v>2001</v>
       </c>
       <c r="G53" t="s">
@@ -2912,16 +2923,16 @@
       <c r="I53">
         <v>1</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K53" t="s">
         <v>130</v>
       </c>
-      <c r="L53">
+      <c r="L53" s="1">
         <v>2</v>
       </c>
-      <c r="M53">
+      <c r="M53" s="1">
         <v>1</v>
       </c>
       <c r="N53" t="s">
@@ -2962,7 +2973,7 @@
       <c r="E54" t="s">
         <v>133</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="1">
         <v>2007</v>
       </c>
       <c r="G54" t="s">
@@ -2974,13 +2985,13 @@
       <c r="I54">
         <v>0</v>
       </c>
-      <c r="J54" t="s">
+      <c r="J54" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L54">
-        <v>0</v>
-      </c>
-      <c r="M54">
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+      <c r="M54" s="1">
         <v>1</v>
       </c>
       <c r="N54" t="s">
@@ -3021,7 +3032,7 @@
       <c r="E55" t="s">
         <v>136</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="1">
         <v>2012</v>
       </c>
       <c r="G55" t="s">
@@ -3033,16 +3044,16 @@
       <c r="I55">
         <v>1</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="1" t="s">
         <v>23</v>
       </c>
       <c r="K55" t="s">
         <v>137</v>
       </c>
-      <c r="L55">
-        <v>0</v>
-      </c>
-      <c r="M55">
+      <c r="L55" s="1">
+        <v>0</v>
+      </c>
+      <c r="M55" s="1">
         <v>1</v>
       </c>
       <c r="N55" t="s">
@@ -3083,7 +3094,7 @@
       <c r="E56" t="s">
         <v>140</v>
       </c>
-      <c r="F56">
+      <c r="F56" s="1">
         <v>2014</v>
       </c>
       <c r="G56" t="s">
@@ -3095,13 +3106,13 @@
       <c r="I56">
         <v>1</v>
       </c>
-      <c r="J56" t="s">
+      <c r="J56" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L56">
+      <c r="L56" s="1">
         <v>2</v>
       </c>
-      <c r="M56">
+      <c r="M56" s="1">
         <v>1</v>
       </c>
       <c r="N56" t="s">
@@ -3142,7 +3153,7 @@
       <c r="E57" t="s">
         <v>144</v>
       </c>
-      <c r="F57">
+      <c r="F57" s="1">
         <v>2015</v>
       </c>
       <c r="G57" t="s">
@@ -3154,13 +3165,13 @@
       <c r="I57">
         <v>0</v>
       </c>
-      <c r="J57" t="s">
+      <c r="J57" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
+      <c r="L57" s="1">
+        <v>0</v>
+      </c>
+      <c r="M57" s="1">
         <v>1</v>
       </c>
       <c r="N57" t="s">
@@ -3201,7 +3212,7 @@
       <c r="E58" t="s">
         <v>148</v>
       </c>
-      <c r="F58">
+      <c r="F58" s="1">
         <v>2018</v>
       </c>
       <c r="G58" t="s">
@@ -3213,13 +3224,13 @@
       <c r="I58">
         <v>0</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J58" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L58">
-        <v>0</v>
-      </c>
-      <c r="M58">
+      <c r="L58" s="1">
+        <v>0</v>
+      </c>
+      <c r="M58" s="1">
         <v>1</v>
       </c>
       <c r="N58" t="s">
@@ -3260,7 +3271,7 @@
       <c r="E59" t="s">
         <v>151</v>
       </c>
-      <c r="F59">
+      <c r="F59" s="1">
         <v>2016</v>
       </c>
       <c r="G59" t="s">
@@ -3272,13 +3283,13 @@
       <c r="I59">
         <v>0</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L59">
-        <v>0</v>
-      </c>
-      <c r="M59">
+      <c r="L59" s="1">
+        <v>0</v>
+      </c>
+      <c r="M59" s="1">
         <v>1</v>
       </c>
       <c r="N59" t="s">
@@ -3319,7 +3330,7 @@
       <c r="E60" t="s">
         <v>156</v>
       </c>
-      <c r="F60">
+      <c r="F60" s="1">
         <v>2020</v>
       </c>
       <c r="G60" t="s">
@@ -3328,16 +3339,16 @@
       <c r="H60">
         <v>1</v>
       </c>
-      <c r="J60" t="s">
+      <c r="J60" s="1" t="s">
         <v>61</v>
       </c>
       <c r="K60" t="s">
         <v>157</v>
       </c>
-      <c r="L60">
+      <c r="L60" s="1">
         <v>3</v>
       </c>
-      <c r="M60">
+      <c r="M60" s="1">
         <v>1</v>
       </c>
       <c r="N60" t="s">
@@ -3378,7 +3389,7 @@
       <c r="E61" t="s">
         <v>161</v>
       </c>
-      <c r="F61">
+      <c r="F61" s="1">
         <v>2017</v>
       </c>
       <c r="G61" t="s">
@@ -3387,16 +3398,16 @@
       <c r="H61">
         <v>1</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K61" t="s">
         <v>163</v>
       </c>
-      <c r="L61">
+      <c r="L61" s="1">
         <v>8</v>
       </c>
-      <c r="M61">
+      <c r="M61" s="1">
         <v>1</v>
       </c>
       <c r="N61" t="s">
@@ -3437,7 +3448,7 @@
       <c r="E62" t="s">
         <v>168</v>
       </c>
-      <c r="F62">
+      <c r="F62" s="1">
         <v>2015</v>
       </c>
       <c r="G62" t="s">
@@ -3446,16 +3457,16 @@
       <c r="H62">
         <v>1</v>
       </c>
-      <c r="J62" t="s">
+      <c r="J62" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K62" t="s">
         <v>169</v>
       </c>
-      <c r="L62">
+      <c r="L62" s="1">
         <v>7</v>
       </c>
-      <c r="M62">
+      <c r="M62" s="1">
         <v>0</v>
       </c>
       <c r="N62" t="s">
@@ -3496,7 +3507,7 @@
       <c r="E63" t="s">
         <v>174</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <v>2012</v>
       </c>
       <c r="G63" t="s">
@@ -3505,16 +3516,16 @@
       <c r="H63">
         <v>1</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K63" t="s">
         <v>175</v>
       </c>
-      <c r="L63">
+      <c r="L63" s="1">
         <v>3</v>
       </c>
-      <c r="M63">
+      <c r="M63" s="1">
         <v>0</v>
       </c>
       <c r="N63" t="s">
@@ -3555,7 +3566,7 @@
       <c r="E64" t="s">
         <v>179</v>
       </c>
-      <c r="F64">
+      <c r="F64" s="1">
         <v>2008</v>
       </c>
       <c r="G64" t="s">
@@ -3564,16 +3575,16 @@
       <c r="H64">
         <v>1</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J64" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K64" t="s">
         <v>180</v>
       </c>
-      <c r="L64">
+      <c r="L64" s="1">
         <v>2</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="1">
         <v>0</v>
       </c>
       <c r="N64" t="s">
@@ -3614,7 +3625,7 @@
       <c r="E65" t="s">
         <v>183</v>
       </c>
-      <c r="F65">
+      <c r="F65" s="1">
         <v>2006</v>
       </c>
       <c r="G65" t="s">
@@ -3623,16 +3634,16 @@
       <c r="H65">
         <v>1</v>
       </c>
-      <c r="J65" t="s">
+      <c r="J65" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K65" t="s">
         <v>184</v>
       </c>
-      <c r="L65">
+      <c r="L65" s="1">
         <v>2</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="1">
         <v>0</v>
       </c>
       <c r="N65" t="s">
@@ -3667,7 +3678,7 @@
       <c r="C66" t="s">
         <v>183</v>
       </c>
-      <c r="F66">
+      <c r="F66" s="1">
         <v>2001</v>
       </c>
       <c r="G66" t="s">
@@ -3676,13 +3687,13 @@
       <c r="H66">
         <v>1</v>
       </c>
-      <c r="J66" t="s">
+      <c r="J66" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="L66">
-        <v>0</v>
-      </c>
-      <c r="M66">
+      <c r="L66" s="1">
+        <v>0</v>
+      </c>
+      <c r="M66" s="1">
         <v>0</v>
       </c>
       <c r="N66" t="s">
@@ -3723,7 +3734,7 @@
       <c r="E67" t="s">
         <v>190</v>
       </c>
-      <c r="F67">
+      <c r="F67" s="1">
         <v>2011</v>
       </c>
       <c r="G67" t="s">
@@ -3732,13 +3743,13 @@
       <c r="H67">
         <v>1</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J67" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K67" t="s">
         <v>191</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="1">
         <v>5</v>
       </c>
       <c r="N67" t="s">
@@ -3779,7 +3790,7 @@
       <c r="E68" t="s">
         <v>196</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <v>2015</v>
       </c>
       <c r="G68" t="s">
@@ -3788,13 +3799,13 @@
       <c r="H68">
         <v>1</v>
       </c>
-      <c r="J68" t="s">
+      <c r="J68" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K68" t="s">
         <v>197</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="1">
         <v>4</v>
       </c>
       <c r="N68" t="s">
@@ -3829,7 +3840,7 @@
       <c r="C69" t="s">
         <v>201</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="1">
         <v>1999</v>
       </c>
       <c r="G69" t="s">
@@ -3838,10 +3849,10 @@
       <c r="H69">
         <v>1</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J69" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="1">
         <v>0</v>
       </c>
       <c r="N69" t="s">
@@ -3879,7 +3890,7 @@
       <c r="C70" t="s">
         <v>206</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="1">
         <v>1999</v>
       </c>
       <c r="G70" t="s">
@@ -3888,13 +3899,13 @@
       <c r="H70">
         <v>1</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J70" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K70" t="s">
         <v>208</v>
       </c>
-      <c r="L70">
+      <c r="L70" s="1">
         <v>1</v>
       </c>
       <c r="N70" t="s">
@@ -3929,7 +3940,7 @@
       <c r="C71" t="s">
         <v>212</v>
       </c>
-      <c r="F71">
+      <c r="F71" s="1">
         <v>2001</v>
       </c>
       <c r="G71" t="s">
@@ -3938,10 +3949,10 @@
       <c r="H71">
         <v>1</v>
       </c>
-      <c r="J71" t="s">
+      <c r="J71" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L71">
+      <c r="L71" s="1">
         <v>0</v>
       </c>
       <c r="N71" t="s">
@@ -3982,7 +3993,7 @@
       <c r="E72" t="s">
         <v>206</v>
       </c>
-      <c r="F72">
+      <c r="F72" s="1">
         <v>2010</v>
       </c>
       <c r="G72" t="s">
@@ -3991,10 +4002,10 @@
       <c r="H72">
         <v>1</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J72" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L72">
+      <c r="L72" s="1">
         <v>0</v>
       </c>
       <c r="N72" t="s">
@@ -4029,7 +4040,7 @@
       <c r="C73" t="s">
         <v>218</v>
       </c>
-      <c r="F73">
+      <c r="F73" s="1">
         <v>2013</v>
       </c>
       <c r="G73" t="s">
@@ -4038,10 +4049,10 @@
       <c r="H73">
         <v>1</v>
       </c>
-      <c r="J73" t="s">
+      <c r="J73" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L73">
+      <c r="L73" s="1">
         <v>0</v>
       </c>
       <c r="N73" t="s">
@@ -4082,7 +4093,7 @@
       <c r="E74" t="s">
         <v>223</v>
       </c>
-      <c r="F74">
+      <c r="F74" s="1">
         <v>2014</v>
       </c>
       <c r="G74" t="s">
@@ -4091,13 +4102,13 @@
       <c r="H74">
         <v>1</v>
       </c>
-      <c r="J74" t="s">
+      <c r="J74" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K74" t="s">
         <v>224</v>
       </c>
-      <c r="L74">
+      <c r="L74" s="1">
         <v>7</v>
       </c>
       <c r="N74" t="s">
@@ -4141,7 +4152,7 @@
       <c r="E75" t="s">
         <v>231</v>
       </c>
-      <c r="F75">
+      <c r="F75" s="1">
         <v>2015</v>
       </c>
       <c r="G75" t="s">
@@ -4150,10 +4161,10 @@
       <c r="H75">
         <v>1</v>
       </c>
-      <c r="J75" t="s">
+      <c r="J75" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L75">
+      <c r="L75" s="1">
         <v>0</v>
       </c>
       <c r="N75" t="s">
@@ -4194,7 +4205,7 @@
       <c r="E76" t="s">
         <v>236</v>
       </c>
-      <c r="F76">
+      <c r="F76" s="1">
         <v>2019</v>
       </c>
       <c r="G76" t="s">
@@ -4203,10 +4214,10 @@
       <c r="H76">
         <v>1</v>
       </c>
-      <c r="J76" t="s">
+      <c r="J76" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L76">
+      <c r="L76" s="1">
         <v>0</v>
       </c>
       <c r="N76" t="s">
@@ -4241,7 +4252,7 @@
       <c r="C77" t="s">
         <v>239</v>
       </c>
-      <c r="F77">
+      <c r="F77" s="1">
         <v>2019</v>
       </c>
       <c r="G77" t="s">
@@ -4250,10 +4261,10 @@
       <c r="H77">
         <v>1</v>
       </c>
-      <c r="J77" t="s">
+      <c r="J77" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L77">
+      <c r="L77" s="1">
         <v>0</v>
       </c>
       <c r="N77" t="s">
@@ -4294,7 +4305,7 @@
       <c r="E78" t="s">
         <v>212</v>
       </c>
-      <c r="F78">
+      <c r="F78" s="1">
         <v>2003</v>
       </c>
       <c r="G78" t="s">
@@ -4303,10 +4314,10 @@
       <c r="H78">
         <v>1</v>
       </c>
-      <c r="J78" t="s">
+      <c r="J78" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="L78">
+      <c r="L78" s="1">
         <v>0</v>
       </c>
       <c r="N78" t="s">
@@ -4341,7 +4352,7 @@
       <c r="C79" t="s">
         <v>245</v>
       </c>
-      <c r="F79">
+      <c r="F79" s="1">
         <v>1973</v>
       </c>
       <c r="G79" t="s">
@@ -4350,16 +4361,16 @@
       <c r="H79">
         <v>1</v>
       </c>
-      <c r="J79" t="s">
+      <c r="J79" s="1" t="s">
         <v>246</v>
       </c>
       <c r="K79" t="s">
         <v>247</v>
       </c>
-      <c r="L79">
-        <v>1</v>
-      </c>
-      <c r="M79">
+      <c r="L79" s="1">
+        <v>1</v>
+      </c>
+      <c r="M79" s="1">
         <v>0</v>
       </c>
       <c r="N79" t="s">
@@ -4400,7 +4411,7 @@
       <c r="E80" t="s">
         <v>252</v>
       </c>
-      <c r="F80">
+      <c r="F80" s="1">
         <v>1996</v>
       </c>
       <c r="G80" t="s">
@@ -4409,16 +4420,16 @@
       <c r="H80">
         <v>1</v>
       </c>
-      <c r="J80" t="s">
+      <c r="J80" s="1" t="s">
         <v>246</v>
       </c>
       <c r="K80" t="s">
         <v>253</v>
       </c>
-      <c r="L80">
+      <c r="L80" s="1">
         <v>3</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="1">
         <v>0</v>
       </c>
       <c r="N80" t="s">
@@ -4453,7 +4464,7 @@
       <c r="C81" t="s">
         <v>252</v>
       </c>
-      <c r="F81">
+      <c r="F81" s="1">
         <v>1995</v>
       </c>
       <c r="G81" t="s">
@@ -4462,13 +4473,13 @@
       <c r="H81">
         <v>1</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J81" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="L81">
-        <v>0</v>
-      </c>
-      <c r="M81">
+      <c r="L81" s="1">
+        <v>0</v>
+      </c>
+      <c r="M81" s="1">
         <v>0</v>
       </c>
       <c r="N81" t="s">
@@ -4509,7 +4520,7 @@
       <c r="E82" t="s">
         <v>251</v>
       </c>
-      <c r="F82">
+      <c r="F82" s="1">
         <v>1997</v>
       </c>
       <c r="G82" t="s">
@@ -4518,13 +4529,13 @@
       <c r="H82">
         <v>1</v>
       </c>
-      <c r="J82" t="s">
+      <c r="J82" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="L82">
-        <v>0</v>
-      </c>
-      <c r="M82">
+      <c r="L82" s="1">
+        <v>0</v>
+      </c>
+      <c r="M82" s="1">
         <v>0</v>
       </c>
       <c r="N82" t="s">
@@ -4565,7 +4576,7 @@
       <c r="E83" t="s">
         <v>265</v>
       </c>
-      <c r="F83">
+      <c r="F83" s="1">
         <v>2007</v>
       </c>
       <c r="G83" t="s">
@@ -4574,16 +4585,16 @@
       <c r="H83">
         <v>1</v>
       </c>
-      <c r="J83" t="s">
+      <c r="J83" s="1" t="s">
         <v>266</v>
       </c>
       <c r="K83" t="s">
         <v>267</v>
       </c>
-      <c r="L83">
-        <v>1</v>
-      </c>
-      <c r="M83">
+      <c r="L83" s="1">
+        <v>1</v>
+      </c>
+      <c r="M83" s="1">
         <v>1</v>
       </c>
       <c r="N83" t="s">
@@ -4624,7 +4635,7 @@
       <c r="E84" t="s">
         <v>265</v>
       </c>
-      <c r="F84">
+      <c r="F84" s="1">
         <v>2006</v>
       </c>
       <c r="G84" t="s">
@@ -4633,13 +4644,13 @@
       <c r="H84">
         <v>1</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J84" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="L84">
-        <v>0</v>
-      </c>
-      <c r="M84">
+      <c r="L84" s="1">
+        <v>0</v>
+      </c>
+      <c r="M84" s="1">
         <v>1</v>
       </c>
       <c r="N84" t="s">
@@ -4680,7 +4691,7 @@
       <c r="E85" t="s">
         <v>274</v>
       </c>
-      <c r="F85">
+      <c r="F85" s="1">
         <v>2015</v>
       </c>
       <c r="G85" t="s">
@@ -4689,13 +4700,13 @@
       <c r="H85">
         <v>1</v>
       </c>
-      <c r="J85" t="s">
+      <c r="J85" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="L85">
-        <v>0</v>
-      </c>
-      <c r="M85">
+      <c r="L85" s="1">
+        <v>0</v>
+      </c>
+      <c r="M85" s="1">
         <v>0</v>
       </c>
       <c r="N85" t="s">
@@ -4736,7 +4747,7 @@
       <c r="E86" t="s">
         <v>274</v>
       </c>
-      <c r="F86">
+      <c r="F86" s="1">
         <v>2015</v>
       </c>
       <c r="G86" t="s">
@@ -4745,13 +4756,13 @@
       <c r="H86">
         <v>1</v>
       </c>
-      <c r="J86" t="s">
+      <c r="J86" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-      <c r="M86">
+      <c r="L86" s="1">
+        <v>0</v>
+      </c>
+      <c r="M86" s="1">
         <v>0</v>
       </c>
       <c r="N86" t="s">
@@ -4792,7 +4803,7 @@
       <c r="E87" t="s">
         <v>260</v>
       </c>
-      <c r="F87">
+      <c r="F87" s="1">
         <v>2005</v>
       </c>
       <c r="G87" t="s">
@@ -4801,16 +4812,16 @@
       <c r="H87">
         <v>1</v>
       </c>
-      <c r="J87" t="s">
+      <c r="J87" s="1" t="s">
         <v>281</v>
       </c>
       <c r="K87" t="s">
         <v>282</v>
       </c>
-      <c r="L87">
+      <c r="L87" s="1">
         <v>2</v>
       </c>
-      <c r="M87">
+      <c r="M87" s="1">
         <v>0</v>
       </c>
       <c r="N87" t="s">
@@ -4851,7 +4862,7 @@
       <c r="E88" t="s">
         <v>286</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="1">
         <v>2013</v>
       </c>
       <c r="G88" t="s">
@@ -4860,13 +4871,13 @@
       <c r="H88">
         <v>1</v>
       </c>
-      <c r="J88" t="s">
+      <c r="J88" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="L88">
-        <v>0</v>
-      </c>
-      <c r="M88">
+      <c r="L88" s="1">
+        <v>0</v>
+      </c>
+      <c r="M88" s="1">
         <v>1</v>
       </c>
       <c r="N88" t="s">
@@ -4907,7 +4918,7 @@
       <c r="E89" t="s">
         <v>292</v>
       </c>
-      <c r="F89">
+      <c r="F89" s="1">
         <v>2016</v>
       </c>
       <c r="G89" t="s">
@@ -4916,16 +4927,16 @@
       <c r="H89">
         <v>1</v>
       </c>
-      <c r="J89" t="s">
+      <c r="J89" s="1" t="s">
         <v>88</v>
       </c>
       <c r="K89" t="s">
         <v>293</v>
       </c>
-      <c r="L89">
-        <v>1</v>
-      </c>
-      <c r="M89">
+      <c r="L89" s="1">
+        <v>1</v>
+      </c>
+      <c r="M89" s="1">
         <v>1</v>
       </c>
       <c r="N89" t="s">
@@ -4960,7 +4971,7 @@
       <c r="C90" t="s">
         <v>296</v>
       </c>
-      <c r="F90">
+      <c r="F90" s="1">
         <v>1957</v>
       </c>
       <c r="G90" t="s">
@@ -4969,13 +4980,13 @@
       <c r="H90">
         <v>1</v>
       </c>
-      <c r="J90" t="s">
+      <c r="J90" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="L90">
-        <v>0</v>
-      </c>
-      <c r="M90">
+      <c r="L90" s="1">
+        <v>0</v>
+      </c>
+      <c r="M90" s="1">
         <v>0</v>
       </c>
       <c r="N90" t="s">
@@ -5010,7 +5021,7 @@
       <c r="C91" t="s">
         <v>300</v>
       </c>
-      <c r="F91">
+      <c r="F91" s="1">
         <v>1949</v>
       </c>
       <c r="G91" t="s">
@@ -5019,13 +5030,13 @@
       <c r="H91">
         <v>1</v>
       </c>
-      <c r="J91" t="s">
+      <c r="J91" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="L91">
-        <v>0</v>
-      </c>
-      <c r="M91">
+      <c r="L91" s="1">
+        <v>0</v>
+      </c>
+      <c r="M91" s="1">
         <v>0</v>
       </c>
       <c r="N91" t="s">
@@ -5060,7 +5071,7 @@
       <c r="C92" t="s">
         <v>304</v>
       </c>
-      <c r="F92">
+      <c r="F92" s="1">
         <v>1982</v>
       </c>
       <c r="G92" t="s">
@@ -5072,13 +5083,13 @@
       <c r="I92">
         <v>0</v>
       </c>
-      <c r="J92" t="s">
+      <c r="J92" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L92">
-        <v>0</v>
-      </c>
-      <c r="M92">
+      <c r="L92" s="1">
+        <v>0</v>
+      </c>
+      <c r="M92" s="1">
         <v>0</v>
       </c>
       <c r="N92" t="s">
@@ -5119,7 +5130,7 @@
       <c r="E93" t="s">
         <v>304</v>
       </c>
-      <c r="F93">
+      <c r="F93" s="1">
         <v>1988</v>
       </c>
       <c r="G93" t="s">
@@ -5131,13 +5142,13 @@
       <c r="I93">
         <v>0</v>
       </c>
-      <c r="J93" t="s">
+      <c r="J93" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L93">
-        <v>0</v>
-      </c>
-      <c r="M93">
+      <c r="L93" s="1">
+        <v>0</v>
+      </c>
+      <c r="M93" s="1">
         <v>0</v>
       </c>
       <c r="N93" t="s">
@@ -5178,7 +5189,7 @@
       <c r="E94" t="s">
         <v>311</v>
       </c>
-      <c r="F94">
+      <c r="F94" s="1">
         <v>1991</v>
       </c>
       <c r="G94" t="s">
@@ -5190,13 +5201,13 @@
       <c r="I94">
         <v>0</v>
       </c>
-      <c r="J94" t="s">
+      <c r="J94" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L94">
-        <v>0</v>
-      </c>
-      <c r="M94">
+      <c r="L94" s="1">
+        <v>0</v>
+      </c>
+      <c r="M94" s="1">
         <v>0</v>
       </c>
       <c r="N94" t="s">
@@ -5237,7 +5248,7 @@
       <c r="E95" t="s">
         <v>314</v>
       </c>
-      <c r="F95">
+      <c r="F95" s="1">
         <v>1991</v>
       </c>
       <c r="G95" t="s">
@@ -5249,13 +5260,13 @@
       <c r="I95">
         <v>0</v>
       </c>
-      <c r="J95" t="s">
+      <c r="J95" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L95">
-        <v>0</v>
-      </c>
-      <c r="M95">
+      <c r="L95" s="1">
+        <v>0</v>
+      </c>
+      <c r="M95" s="1">
         <v>0</v>
       </c>
       <c r="N95" t="s">
@@ -5296,7 +5307,7 @@
       <c r="E96" t="s">
         <v>318</v>
       </c>
-      <c r="F96">
+      <c r="F96" s="1">
         <v>1994</v>
       </c>
       <c r="G96" t="s">
@@ -5308,16 +5319,16 @@
       <c r="I96">
         <v>0</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J96" s="1" t="s">
         <v>110</v>
       </c>
       <c r="K96" t="s">
         <v>24</v>
       </c>
-      <c r="L96">
-        <v>1</v>
-      </c>
-      <c r="M96">
+      <c r="L96" s="1">
+        <v>1</v>
+      </c>
+      <c r="M96" s="1">
         <v>0</v>
       </c>
       <c r="N96" t="s">
@@ -5358,7 +5369,7 @@
       <c r="E97" t="s">
         <v>320</v>
       </c>
-      <c r="F97">
+      <c r="F97" s="1">
         <v>1994</v>
       </c>
       <c r="G97" t="s">
@@ -5370,13 +5381,13 @@
       <c r="I97">
         <v>0</v>
       </c>
-      <c r="J97" t="s">
+      <c r="J97" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L97">
-        <v>0</v>
-      </c>
-      <c r="M97">
+      <c r="L97" s="1">
+        <v>0</v>
+      </c>
+      <c r="M97" s="1">
         <v>0</v>
       </c>
       <c r="N97" t="s">
@@ -5417,7 +5428,7 @@
       <c r="E98" t="s">
         <v>119</v>
       </c>
-      <c r="F98">
+      <c r="F98" s="1">
         <v>1994</v>
       </c>
       <c r="G98" t="s">
@@ -5429,13 +5440,13 @@
       <c r="I98">
         <v>0</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J98" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="L98">
-        <v>0</v>
-      </c>
-      <c r="M98">
+      <c r="L98" s="1">
+        <v>0</v>
+      </c>
+      <c r="M98" s="1">
         <v>0</v>
       </c>
       <c r="N98" t="s">
@@ -5470,13 +5481,13 @@
       <c r="C99" t="s">
         <v>325</v>
       </c>
-      <c r="F99">
+      <c r="F99" s="1">
         <v>2011</v>
       </c>
       <c r="H99">
         <v>0</v>
       </c>
-      <c r="L99">
+      <c r="L99" s="1">
         <v>0</v>
       </c>
       <c r="U99">
@@ -5496,13 +5507,13 @@
       <c r="E100" t="s">
         <v>327</v>
       </c>
-      <c r="F100">
+      <c r="F100" s="1">
         <v>2007</v>
       </c>
       <c r="H100">
         <v>0</v>
       </c>
-      <c r="L100">
+      <c r="L100" s="1">
         <v>0</v>
       </c>
       <c r="U100">
@@ -5519,13 +5530,13 @@
       <c r="C101" t="s">
         <v>113</v>
       </c>
-      <c r="F101">
+      <c r="F101" s="1">
         <v>1984</v>
       </c>
       <c r="H101">
         <v>0</v>
       </c>
-      <c r="L101">
+      <c r="L101" s="1">
         <v>0</v>
       </c>
       <c r="U101">
@@ -5542,13 +5553,13 @@
       <c r="C102" t="s">
         <v>330</v>
       </c>
-      <c r="F102">
+      <c r="F102" s="1">
         <v>1990</v>
       </c>
       <c r="H102">
         <v>0</v>
       </c>
-      <c r="L102">
+      <c r="L102" s="1">
         <v>0</v>
       </c>
       <c r="U102">

</xml_diff>